<commit_message>
exproting new bom from dxf uses more tags of excell table
</commit_message>
<xml_diff>
--- a/tests/test1/BOM_1.1_updated.xlsx
+++ b/tests/test1/BOM_1.1_updated.xlsx
@@ -3,21 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1848" yWindow="648" windowWidth="17280" windowHeight="8964" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BOM" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="A">#REF!</definedName>
-    <definedName name="DBWBOM" localSheetId="0">#REF!</definedName>
     <definedName name="DBWBOM">#REF!</definedName>
-    <definedName name="DBWBUY" localSheetId="0">#REF!</definedName>
     <definedName name="DBWBUY">#REF!</definedName>
-    <definedName name="DBWTREE" localSheetId="0">#REF!</definedName>
     <definedName name="DBWTREE">#REF!</definedName>
     <definedName name="Dint">#REF!</definedName>
-    <definedName name="ELCADExport" localSheetId="0">BOM!$B$1:$Q$1</definedName>
     <definedName name="ELCADExport">#REF!</definedName>
     <definedName name="erel">#REF!</definedName>
     <definedName name="jaar">#REF!</definedName>
@@ -26,6 +22,10 @@
     <definedName name="Q">#REF!</definedName>
     <definedName name="Re">#REF!</definedName>
     <definedName name="v">#REF!</definedName>
+    <definedName name="DBWBOM" localSheetId="0">#REF!</definedName>
+    <definedName name="DBWBUY" localSheetId="0">#REF!</definedName>
+    <definedName name="DBWTREE" localSheetId="0">#REF!</definedName>
+    <definedName name="ELCADExport" localSheetId="0">BOM!$B$1:$Q$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'BOM'!$A$1:$AJ$38</definedName>
   </definedNames>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -37,7 +37,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -124,8 +124,13 @@
       <u val="single"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="8"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -140,14 +145,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FF0000"/>
-        <bgColor rgb="00FF0000"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00CCCCCC"/>
-        <bgColor rgb="00CCCCCC"/>
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
       </patternFill>
     </fill>
   </fills>
@@ -200,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -274,9 +285,6 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -312,6 +320,24 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -596,10 +622,10 @@
   <dimension ref="A1:AH45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="L18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -801,61 +827,69 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="14.4" customFormat="1" customHeight="1" s="28">
-      <c r="A2" s="29" t="n">
+    <row r="2" ht="14.4" customFormat="1" customHeight="1" s="27">
+      <c r="A2" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="inlineStr">
+      <c r="B2" s="28" t="inlineStr">
         <is>
           <t>CH</t>
         </is>
       </c>
-      <c r="C2" s="29" t="n">
+      <c r="C2" s="28" t="n">
         <v>905</v>
       </c>
-      <c r="D2" s="29" t="inlineStr"/>
-      <c r="E2" s="30" t="inlineStr">
+      <c r="D2" s="28" t="n"/>
+      <c r="E2" s="29" t="inlineStr">
         <is>
           <t>CH905</t>
         </is>
       </c>
-      <c r="F2" s="29" t="inlineStr"/>
-      <c r="G2" s="29" t="inlineStr"/>
-      <c r="H2" s="29" t="inlineStr"/>
-      <c r="I2" s="29" t="inlineStr"/>
-      <c r="J2" s="29" t="inlineStr"/>
-      <c r="K2" s="29" t="inlineStr"/>
-      <c r="L2" s="29" t="inlineStr"/>
-      <c r="M2" s="31" t="inlineStr">
+      <c r="F2" s="28" t="n"/>
+      <c r="G2" s="28" t="n"/>
+      <c r="H2" s="28" t="n"/>
+      <c r="I2" s="28" t="n"/>
+      <c r="J2" s="28" t="n"/>
+      <c r="K2" s="28" t="n"/>
+      <c r="L2" s="28" t="n"/>
+      <c r="M2" s="30" t="inlineStr">
         <is>
           <t>Chiller</t>
         </is>
       </c>
-      <c r="N2" s="31" t="inlineStr">
+      <c r="N2" s="30" t="inlineStr">
         <is>
           <t>Chiller</t>
         </is>
       </c>
-      <c r="O2" s="29" t="inlineStr"/>
-      <c r="P2" s="31" t="inlineStr"/>
-      <c r="Q2" s="32" t="inlineStr"/>
-      <c r="R2" s="29" t="inlineStr"/>
-      <c r="S2" s="29" t="inlineStr"/>
-      <c r="T2" s="29" t="inlineStr"/>
-      <c r="U2" s="29" t="n"/>
-      <c r="V2" s="29" t="inlineStr"/>
-      <c r="W2" s="29" t="inlineStr"/>
-      <c r="X2" s="31" t="inlineStr"/>
-      <c r="Y2" s="31" t="inlineStr"/>
-      <c r="Z2" s="33" t="inlineStr"/>
-      <c r="AA2" s="31" t="inlineStr"/>
-      <c r="AB2" s="29" t="inlineStr"/>
-      <c r="AC2" s="29" t="inlineStr"/>
-      <c r="AD2" s="31" t="inlineStr"/>
-      <c r="AE2" s="31" t="inlineStr"/>
-      <c r="AF2" s="31" t="inlineStr"/>
-      <c r="AG2" s="29" t="inlineStr"/>
-      <c r="AH2" s="34" t="inlineStr"/>
+      <c r="O2" s="28" t="inlineStr">
+        <is>
+          <t>AISI316</t>
+        </is>
+      </c>
+      <c r="P2" s="30" t="n"/>
+      <c r="Q2" s="31" t="n"/>
+      <c r="R2" s="28" t="n"/>
+      <c r="S2" s="28" t="n"/>
+      <c r="T2" s="28" t="n"/>
+      <c r="U2" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
+      <c r="V2" s="28" t="n"/>
+      <c r="W2" s="28" t="n"/>
+      <c r="X2" s="30" t="n"/>
+      <c r="Y2" s="30" t="n"/>
+      <c r="Z2" s="32" t="n"/>
+      <c r="AA2" s="30" t="n"/>
+      <c r="AB2" s="28" t="n"/>
+      <c r="AC2" s="28" t="n"/>
+      <c r="AD2" s="30" t="n"/>
+      <c r="AE2" s="30" t="n"/>
+      <c r="AF2" s="30" t="n"/>
+      <c r="AG2" s="28" t="n"/>
+      <c r="AH2" s="33" t="n"/>
     </row>
     <row r="3" ht="14.4" customHeight="1">
       <c r="A3" s="10" t="n">
@@ -892,13 +926,21 @@
           <t>Chiller</t>
         </is>
       </c>
-      <c r="O3" s="10" t="n"/>
+      <c r="O3" s="28" t="inlineStr">
+        <is>
+          <t>AISI317</t>
+        </is>
+      </c>
       <c r="P3" s="13" t="n"/>
       <c r="Q3" s="18" t="n"/>
       <c r="R3" s="10" t="n"/>
       <c r="S3" s="10" t="n"/>
       <c r="T3" s="10" t="n"/>
-      <c r="U3" s="10" t="n"/>
+      <c r="U3" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V3" s="10" t="n"/>
       <c r="W3" s="10" t="n"/>
       <c r="X3" s="13" t="n"/>
@@ -948,13 +990,21 @@
           <t>Vasca Satinatura</t>
         </is>
       </c>
-      <c r="O4" s="10" t="n"/>
+      <c r="O4" s="28" t="inlineStr">
+        <is>
+          <t>AISI318</t>
+        </is>
+      </c>
       <c r="P4" s="13" t="n"/>
       <c r="Q4" s="18" t="n"/>
       <c r="R4" s="10" t="n"/>
       <c r="S4" s="10" t="n"/>
       <c r="T4" s="10" t="n"/>
-      <c r="U4" s="10" t="n"/>
+      <c r="U4" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V4" s="10" t="n"/>
       <c r="W4" s="10" t="n"/>
       <c r="X4" s="13" t="n"/>
@@ -1004,13 +1054,21 @@
           <t>Vasca Stoccaggio</t>
         </is>
       </c>
-      <c r="O5" s="10" t="n"/>
+      <c r="O5" s="28" t="inlineStr">
+        <is>
+          <t>AISI319</t>
+        </is>
+      </c>
       <c r="P5" s="13" t="n"/>
       <c r="Q5" s="18" t="n"/>
       <c r="R5" s="10" t="n"/>
       <c r="S5" s="10" t="n"/>
       <c r="T5" s="10" t="n"/>
-      <c r="U5" s="10" t="n"/>
+      <c r="U5" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V5" s="10" t="n"/>
       <c r="W5" s="10" t="n"/>
       <c r="X5" s="13" t="n"/>
@@ -1060,13 +1118,21 @@
           <t>Vasca Stoccaggio</t>
         </is>
       </c>
-      <c r="O6" s="10" t="n"/>
+      <c r="O6" s="28" t="inlineStr">
+        <is>
+          <t>AISI320</t>
+        </is>
+      </c>
       <c r="P6" s="13" t="n"/>
       <c r="Q6" s="18" t="n"/>
       <c r="R6" s="10" t="n"/>
       <c r="S6" s="10" t="n"/>
       <c r="T6" s="10" t="n"/>
-      <c r="U6" s="10" t="n"/>
+      <c r="U6" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V6" s="10" t="n"/>
       <c r="W6" s="10" t="n"/>
       <c r="X6" s="13" t="n"/>
@@ -1116,13 +1182,21 @@
           <t>Serbatoi stoccaggio</t>
         </is>
       </c>
-      <c r="O7" s="10" t="n"/>
+      <c r="O7" s="28" t="inlineStr">
+        <is>
+          <t>AISI321</t>
+        </is>
+      </c>
       <c r="P7" s="13" t="n"/>
       <c r="Q7" s="18" t="n"/>
       <c r="R7" s="10" t="n"/>
       <c r="S7" s="10" t="n"/>
       <c r="T7" s="10" t="n"/>
-      <c r="U7" s="10" t="n"/>
+      <c r="U7" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V7" s="10" t="n"/>
       <c r="W7" s="10" t="n"/>
       <c r="X7" s="13" t="n"/>
@@ -1172,13 +1246,21 @@
           <t>Serbatoio di refluo contenente ammoniaca</t>
         </is>
       </c>
-      <c r="O8" s="10" t="n"/>
+      <c r="O8" s="28" t="inlineStr">
+        <is>
+          <t>AISI322</t>
+        </is>
+      </c>
       <c r="P8" s="13" t="n"/>
       <c r="Q8" s="18" t="n"/>
       <c r="R8" s="10" t="n"/>
       <c r="S8" s="10" t="n"/>
       <c r="T8" s="10" t="n"/>
-      <c r="U8" s="10" t="n"/>
+      <c r="U8" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V8" s="10" t="n"/>
       <c r="W8" s="10" t="n"/>
       <c r="X8" s="13" t="n"/>
@@ -1228,13 +1310,21 @@
           <t>Torre di strippaggio</t>
         </is>
       </c>
-      <c r="O9" s="10" t="n"/>
+      <c r="O9" s="28" t="inlineStr">
+        <is>
+          <t>AISI323</t>
+        </is>
+      </c>
       <c r="P9" s="13" t="n"/>
       <c r="Q9" s="18" t="n"/>
       <c r="R9" s="10" t="n"/>
       <c r="S9" s="10" t="n"/>
       <c r="T9" s="10" t="n"/>
-      <c r="U9" s="10" t="n"/>
+      <c r="U9" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V9" s="10" t="n"/>
       <c r="W9" s="10" t="n"/>
       <c r="X9" s="13" t="n"/>
@@ -1282,13 +1372,21 @@
         </is>
       </c>
       <c r="N10" s="13" t="n"/>
-      <c r="O10" s="10" t="n"/>
+      <c r="O10" s="28" t="inlineStr">
+        <is>
+          <t>AISI324</t>
+        </is>
+      </c>
       <c r="P10" s="13" t="n"/>
       <c r="Q10" s="18" t="n"/>
       <c r="R10" s="10" t="n"/>
       <c r="S10" s="10" t="n"/>
       <c r="T10" s="10" t="n"/>
-      <c r="U10" s="10" t="n"/>
+      <c r="U10" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V10" s="10" t="n"/>
       <c r="W10" s="10" t="n"/>
       <c r="X10" s="13" t="n"/>
@@ -1338,13 +1436,21 @@
           <t>Pompa a Cavità progressiva</t>
         </is>
       </c>
-      <c r="O11" s="10" t="n"/>
+      <c r="O11" s="28" t="inlineStr">
+        <is>
+          <t>AISI325</t>
+        </is>
+      </c>
       <c r="P11" s="13" t="n"/>
       <c r="Q11" s="18" t="n"/>
       <c r="R11" s="10" t="n"/>
       <c r="S11" s="10" t="n"/>
       <c r="T11" s="10" t="n"/>
-      <c r="U11" s="10" t="n"/>
+      <c r="U11" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V11" s="10" t="n"/>
       <c r="W11" s="10" t="n"/>
       <c r="X11" s="13" t="n"/>
@@ -1394,13 +1500,21 @@
           <t>Filtropressa</t>
         </is>
       </c>
-      <c r="O12" s="10" t="n"/>
+      <c r="O12" s="28" t="inlineStr">
+        <is>
+          <t>AISI326</t>
+        </is>
+      </c>
       <c r="P12" s="13" t="n"/>
       <c r="Q12" s="18" t="n"/>
       <c r="R12" s="10" t="n"/>
       <c r="S12" s="10" t="n"/>
       <c r="T12" s="10" t="n"/>
-      <c r="U12" s="10" t="n"/>
+      <c r="U12" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V12" s="10" t="n"/>
       <c r="W12" s="10" t="n"/>
       <c r="X12" s="13" t="n"/>
@@ -1450,13 +1564,21 @@
           <t>Screw Conveyor</t>
         </is>
       </c>
-      <c r="O13" s="10" t="n"/>
+      <c r="O13" s="28" t="inlineStr">
+        <is>
+          <t>AISI327</t>
+        </is>
+      </c>
       <c r="P13" s="13" t="n"/>
       <c r="Q13" s="18" t="n"/>
       <c r="R13" s="10" t="n"/>
       <c r="S13" s="10" t="n"/>
       <c r="T13" s="10" t="n"/>
-      <c r="U13" s="10" t="n"/>
+      <c r="U13" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V13" s="10" t="n"/>
       <c r="W13" s="10" t="n"/>
       <c r="X13" s="13" t="n"/>
@@ -1506,13 +1628,21 @@
           <t>Abattitore</t>
         </is>
       </c>
-      <c r="O14" s="10" t="n"/>
+      <c r="O14" s="28" t="inlineStr">
+        <is>
+          <t>AISI328</t>
+        </is>
+      </c>
       <c r="P14" s="13" t="n"/>
       <c r="Q14" s="18" t="n"/>
       <c r="R14" s="10" t="n"/>
       <c r="S14" s="10" t="n"/>
       <c r="T14" s="10" t="n"/>
-      <c r="U14" s="10" t="n"/>
+      <c r="U14" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V14" s="10" t="n"/>
       <c r="W14" s="10" t="n"/>
       <c r="X14" s="13" t="n"/>
@@ -1562,13 +1692,21 @@
           <t>Pompa a Cavità progressiva</t>
         </is>
       </c>
-      <c r="O15" s="10" t="n"/>
+      <c r="O15" s="28" t="inlineStr">
+        <is>
+          <t>AISI329</t>
+        </is>
+      </c>
       <c r="P15" s="13" t="n"/>
       <c r="Q15" s="18" t="n"/>
       <c r="R15" s="10" t="n"/>
       <c r="S15" s="10" t="n"/>
       <c r="T15" s="10" t="n"/>
-      <c r="U15" s="10" t="n"/>
+      <c r="U15" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V15" s="10" t="n"/>
       <c r="W15" s="10" t="n"/>
       <c r="X15" s="13" t="n"/>
@@ -1618,13 +1756,21 @@
           <t>Filtropressa</t>
         </is>
       </c>
-      <c r="O16" s="10" t="n"/>
+      <c r="O16" s="28" t="inlineStr">
+        <is>
+          <t>AISI330</t>
+        </is>
+      </c>
       <c r="P16" s="13" t="n"/>
       <c r="Q16" s="18" t="n"/>
       <c r="R16" s="10" t="n"/>
       <c r="S16" s="10" t="n"/>
       <c r="T16" s="10" t="n"/>
-      <c r="U16" s="10" t="n"/>
+      <c r="U16" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V16" s="10" t="n"/>
       <c r="W16" s="10" t="n"/>
       <c r="X16" s="13" t="n"/>
@@ -1674,13 +1820,21 @@
           <t>Pompa dosatrice</t>
         </is>
       </c>
-      <c r="O17" s="10" t="n"/>
+      <c r="O17" s="28" t="inlineStr">
+        <is>
+          <t>AISI331</t>
+        </is>
+      </c>
       <c r="P17" s="13" t="n"/>
       <c r="Q17" s="18" t="n"/>
       <c r="R17" s="10" t="n"/>
       <c r="S17" s="10" t="n"/>
       <c r="T17" s="10" t="n"/>
-      <c r="U17" s="10" t="n"/>
+      <c r="U17" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V17" s="10" t="n"/>
       <c r="W17" s="10" t="n"/>
       <c r="X17" s="13" t="n"/>
@@ -1730,13 +1884,21 @@
           <t>Pompa chiller</t>
         </is>
       </c>
-      <c r="O18" s="10" t="n"/>
+      <c r="O18" s="28" t="inlineStr">
+        <is>
+          <t>AISI332</t>
+        </is>
+      </c>
       <c r="P18" s="13" t="n"/>
       <c r="Q18" s="18" t="n"/>
       <c r="R18" s="10" t="n"/>
       <c r="S18" s="10" t="n"/>
       <c r="T18" s="10" t="n"/>
-      <c r="U18" s="10" t="n"/>
+      <c r="U18" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V18" s="10" t="n"/>
       <c r="W18" s="10" t="n"/>
       <c r="X18" s="13" t="n"/>
@@ -1786,13 +1948,21 @@
           <t>Pompa dosatrice</t>
         </is>
       </c>
-      <c r="O19" s="10" t="n"/>
+      <c r="O19" s="28" t="inlineStr">
+        <is>
+          <t>AISI333</t>
+        </is>
+      </c>
       <c r="P19" s="13" t="n"/>
       <c r="Q19" s="18" t="n"/>
       <c r="R19" s="10" t="n"/>
       <c r="S19" s="10" t="n"/>
       <c r="T19" s="10" t="n"/>
-      <c r="U19" s="10" t="n"/>
+      <c r="U19" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V19" s="10" t="n"/>
       <c r="W19" s="10" t="n"/>
       <c r="X19" s="13" t="n"/>
@@ -1842,13 +2012,21 @@
           <t>Riscaldatore</t>
         </is>
       </c>
-      <c r="O20" s="10" t="n"/>
+      <c r="O20" s="28" t="inlineStr">
+        <is>
+          <t>AISI334</t>
+        </is>
+      </c>
       <c r="P20" s="13" t="n"/>
       <c r="Q20" s="18" t="n"/>
       <c r="R20" s="10" t="n"/>
       <c r="S20" s="10" t="n"/>
       <c r="T20" s="10" t="n"/>
-      <c r="U20" s="10" t="n"/>
+      <c r="U20" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V20" s="10" t="n"/>
       <c r="W20" s="10" t="n"/>
       <c r="X20" s="13" t="n"/>
@@ -1898,13 +2076,21 @@
           <t>Heater Exchanger</t>
         </is>
       </c>
-      <c r="O21" s="10" t="n"/>
+      <c r="O21" s="28" t="inlineStr">
+        <is>
+          <t>AISI335</t>
+        </is>
+      </c>
       <c r="P21" s="13" t="n"/>
       <c r="Q21" s="18" t="n"/>
       <c r="R21" s="10" t="n"/>
       <c r="S21" s="10" t="n"/>
       <c r="T21" s="10" t="n"/>
-      <c r="U21" s="10" t="n"/>
+      <c r="U21" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V21" s="10" t="n"/>
       <c r="W21" s="10" t="n"/>
       <c r="X21" s="13" t="n"/>
@@ -1954,13 +2140,21 @@
           <t>Gorgoliatore</t>
         </is>
       </c>
-      <c r="O22" s="10" t="n"/>
+      <c r="O22" s="28" t="inlineStr">
+        <is>
+          <t>AISI336</t>
+        </is>
+      </c>
       <c r="P22" s="13" t="n"/>
       <c r="Q22" s="18" t="n"/>
       <c r="R22" s="10" t="n"/>
       <c r="S22" s="10" t="n"/>
       <c r="T22" s="10" t="n"/>
-      <c r="U22" s="10" t="n"/>
+      <c r="U22" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V22" s="10" t="n"/>
       <c r="W22" s="10" t="n"/>
       <c r="X22" s="13" t="n"/>
@@ -2008,13 +2202,21 @@
         </is>
       </c>
       <c r="N23" s="13" t="n"/>
-      <c r="O23" s="10" t="n"/>
+      <c r="O23" s="28" t="inlineStr">
+        <is>
+          <t>AISI337</t>
+        </is>
+      </c>
       <c r="P23" s="13" t="n"/>
       <c r="Q23" s="18" t="n"/>
       <c r="R23" s="10" t="n"/>
       <c r="S23" s="10" t="n"/>
       <c r="T23" s="10" t="n"/>
-      <c r="U23" s="10" t="n"/>
+      <c r="U23" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V23" s="10" t="n"/>
       <c r="W23" s="10" t="n"/>
       <c r="X23" s="13" t="n"/>
@@ -2062,13 +2264,21 @@
         </is>
       </c>
       <c r="N24" s="13" t="n"/>
-      <c r="O24" s="10" t="n"/>
+      <c r="O24" s="28" t="inlineStr">
+        <is>
+          <t>AISI338</t>
+        </is>
+      </c>
       <c r="P24" s="13" t="n"/>
       <c r="Q24" s="18" t="n"/>
       <c r="R24" s="10" t="n"/>
       <c r="S24" s="10" t="n"/>
       <c r="T24" s="10" t="n"/>
-      <c r="U24" s="10" t="n"/>
+      <c r="U24" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V24" s="10" t="n"/>
       <c r="W24" s="10" t="n"/>
       <c r="X24" s="13" t="n"/>
@@ -2116,13 +2326,21 @@
         </is>
       </c>
       <c r="N25" s="13" t="n"/>
-      <c r="O25" s="10" t="n"/>
+      <c r="O25" s="28" t="inlineStr">
+        <is>
+          <t>AISI339</t>
+        </is>
+      </c>
       <c r="P25" s="13" t="n"/>
       <c r="Q25" s="18" t="n"/>
       <c r="R25" s="10" t="n"/>
       <c r="S25" s="10" t="n"/>
       <c r="T25" s="10" t="n"/>
-      <c r="U25" s="10" t="n"/>
+      <c r="U25" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V25" s="10" t="n"/>
       <c r="W25" s="10" t="n"/>
       <c r="X25" s="13" t="n"/>
@@ -2170,13 +2388,21 @@
         </is>
       </c>
       <c r="N26" s="13" t="n"/>
-      <c r="O26" s="10" t="n"/>
+      <c r="O26" s="28" t="inlineStr">
+        <is>
+          <t>AISI340</t>
+        </is>
+      </c>
       <c r="P26" s="13" t="n"/>
       <c r="Q26" s="18" t="n"/>
       <c r="R26" s="10" t="n"/>
       <c r="S26" s="10" t="n"/>
       <c r="T26" s="10" t="n"/>
-      <c r="U26" s="10" t="n"/>
+      <c r="U26" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V26" s="10" t="n"/>
       <c r="W26" s="10" t="n"/>
       <c r="X26" s="13" t="n"/>
@@ -2224,13 +2450,21 @@
         </is>
       </c>
       <c r="N27" s="13" t="n"/>
-      <c r="O27" s="10" t="n"/>
+      <c r="O27" s="28" t="inlineStr">
+        <is>
+          <t>AISI341</t>
+        </is>
+      </c>
       <c r="P27" s="13" t="n"/>
       <c r="Q27" s="18" t="n"/>
       <c r="R27" s="10" t="n"/>
       <c r="S27" s="10" t="n"/>
       <c r="T27" s="10" t="n"/>
-      <c r="U27" s="10" t="n"/>
+      <c r="U27" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V27" s="10" t="n"/>
       <c r="W27" s="10" t="n"/>
       <c r="X27" s="13" t="n"/>
@@ -2278,13 +2512,21 @@
         </is>
       </c>
       <c r="N28" s="13" t="n"/>
-      <c r="O28" s="10" t="n"/>
+      <c r="O28" s="28" t="inlineStr">
+        <is>
+          <t>AISI342</t>
+        </is>
+      </c>
       <c r="P28" s="13" t="n"/>
       <c r="Q28" s="18" t="n"/>
       <c r="R28" s="10" t="n"/>
       <c r="S28" s="10" t="n"/>
       <c r="T28" s="10" t="n"/>
-      <c r="U28" s="10" t="n"/>
+      <c r="U28" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V28" s="10" t="n"/>
       <c r="W28" s="10" t="n"/>
       <c r="X28" s="13" t="n"/>
@@ -2332,13 +2574,21 @@
         </is>
       </c>
       <c r="N29" s="13" t="n"/>
-      <c r="O29" s="10" t="n"/>
+      <c r="O29" s="28" t="inlineStr">
+        <is>
+          <t>AISI343</t>
+        </is>
+      </c>
       <c r="P29" s="13" t="n"/>
       <c r="Q29" s="18" t="n"/>
       <c r="R29" s="10" t="n"/>
       <c r="S29" s="10" t="n"/>
       <c r="T29" s="10" t="n"/>
-      <c r="U29" s="10" t="n"/>
+      <c r="U29" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V29" s="10" t="n"/>
       <c r="W29" s="10" t="n"/>
       <c r="X29" s="13" t="n"/>
@@ -2386,13 +2636,21 @@
         </is>
       </c>
       <c r="N30" s="13" t="n"/>
-      <c r="O30" s="10" t="n"/>
+      <c r="O30" s="28" t="inlineStr">
+        <is>
+          <t>AISI344</t>
+        </is>
+      </c>
       <c r="P30" s="13" t="n"/>
       <c r="Q30" s="18" t="n"/>
       <c r="R30" s="10" t="n"/>
       <c r="S30" s="10" t="n"/>
       <c r="T30" s="10" t="n"/>
-      <c r="U30" s="10" t="n"/>
+      <c r="U30" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V30" s="10" t="n"/>
       <c r="W30" s="10" t="n"/>
       <c r="X30" s="13" t="n"/>
@@ -2440,13 +2698,21 @@
         </is>
       </c>
       <c r="N31" s="13" t="n"/>
-      <c r="O31" s="10" t="n"/>
+      <c r="O31" s="28" t="inlineStr">
+        <is>
+          <t>AISI345</t>
+        </is>
+      </c>
       <c r="P31" s="13" t="n"/>
       <c r="Q31" s="18" t="n"/>
       <c r="R31" s="10" t="n"/>
       <c r="S31" s="10" t="n"/>
       <c r="T31" s="10" t="n"/>
-      <c r="U31" s="10" t="n"/>
+      <c r="U31" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V31" s="10" t="n"/>
       <c r="W31" s="10" t="n"/>
       <c r="X31" s="13" t="n"/>
@@ -2494,13 +2760,21 @@
         </is>
       </c>
       <c r="N32" s="13" t="n"/>
-      <c r="O32" s="10" t="n"/>
+      <c r="O32" s="28" t="inlineStr">
+        <is>
+          <t>AISI346</t>
+        </is>
+      </c>
       <c r="P32" s="13" t="n"/>
       <c r="Q32" s="18" t="n"/>
       <c r="R32" s="10" t="n"/>
       <c r="S32" s="10" t="n"/>
       <c r="T32" s="10" t="n"/>
-      <c r="U32" s="10" t="n"/>
+      <c r="U32" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V32" s="10" t="n"/>
       <c r="W32" s="10" t="n"/>
       <c r="X32" s="13" t="n"/>
@@ -2516,110 +2790,110 @@
       <c r="AH32" s="8" t="n"/>
     </row>
     <row r="33" ht="14.4" customHeight="1">
-      <c r="A33" s="35" t="n">
+      <c r="A33" s="40" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="35" t="inlineStr">
+      <c r="B33" s="40" t="inlineStr">
         <is>
           <t>TE</t>
         </is>
       </c>
-      <c r="C33" s="35" t="n">
+      <c r="C33" s="40" t="n">
         <v>141</v>
       </c>
-      <c r="D33" s="35" t="n"/>
-      <c r="E33" s="36" t="inlineStr">
+      <c r="D33" s="40" t="n"/>
+      <c r="E33" s="41" t="inlineStr">
         <is>
           <t>TE141</t>
         </is>
       </c>
-      <c r="F33" s="35" t="inlineStr">
+      <c r="F33" s="40" t="inlineStr">
         <is>
           <t>Nitrogen</t>
         </is>
       </c>
-      <c r="G33" s="35" t="inlineStr">
+      <c r="G33" s="40" t="inlineStr">
         <is>
           <t>D200</t>
         </is>
       </c>
-      <c r="H33" s="35" t="n"/>
-      <c r="I33" s="35" t="n"/>
-      <c r="J33" s="35" t="n"/>
-      <c r="K33" s="35" t="n"/>
-      <c r="L33" s="35" t="inlineStr">
+      <c r="H33" s="40" t="n"/>
+      <c r="I33" s="40" t="n"/>
+      <c r="J33" s="40" t="n"/>
+      <c r="K33" s="40" t="n"/>
+      <c r="L33" s="40" t="inlineStr">
         <is>
           <t>2_3_4</t>
         </is>
       </c>
-      <c r="M33" s="37" t="inlineStr">
+      <c r="M33" s="42" t="inlineStr">
         <is>
           <t>Temperature probe</t>
         </is>
       </c>
-      <c r="N33" s="37" t="inlineStr">
+      <c r="N33" s="42" t="inlineStr">
         <is>
           <t>Nitrogen heating after E140</t>
         </is>
       </c>
-      <c r="O33" s="35" t="inlineStr">
+      <c r="O33" s="40" t="inlineStr">
         <is>
           <t>AISI316</t>
         </is>
       </c>
-      <c r="P33" s="37" t="inlineStr">
+      <c r="P33" s="42" t="inlineStr">
         <is>
           <t>FKM</t>
         </is>
       </c>
-      <c r="Q33" s="38" t="inlineStr">
+      <c r="Q33" s="43" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="R33" s="35" t="n">
+      <c r="R33" s="40" t="n">
         <v>3</v>
       </c>
-      <c r="S33" s="35" t="n"/>
-      <c r="T33" s="35" t="n"/>
-      <c r="U33" s="35" t="inlineStr">
+      <c r="S33" s="40" t="n"/>
+      <c r="T33" s="40" t="n"/>
+      <c r="U33" s="40" t="inlineStr">
         <is>
           <t>Gas M</t>
         </is>
       </c>
-      <c r="V33" s="35" t="inlineStr">
+      <c r="V33" s="40" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="W33" s="35" t="inlineStr">
+      <c r="W33" s="40" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="X33" s="37" t="inlineStr">
+      <c r="X33" s="42" t="inlineStr">
         <is>
           <t xml:space="preserve">Metron </t>
         </is>
       </c>
-      <c r="Y33" s="37" t="n"/>
-      <c r="Z33" s="39" t="n"/>
-      <c r="AA33" s="37" t="inlineStr">
+      <c r="Y33" s="42" t="n"/>
+      <c r="Z33" s="44" t="n"/>
+      <c r="AA33" s="42" t="inlineStr">
         <is>
           <t>Probe length: 80mm after thread</t>
         </is>
       </c>
-      <c r="AB33" s="35" t="inlineStr">
+      <c r="AB33" s="40" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="AC33" s="35" t="n"/>
-      <c r="AD33" s="37" t="n"/>
-      <c r="AE33" s="37" t="n"/>
-      <c r="AF33" s="37" t="n"/>
-      <c r="AG33" s="35" t="n"/>
-      <c r="AH33" s="40" t="n"/>
+      <c r="AC33" s="40" t="n"/>
+      <c r="AD33" s="42" t="n"/>
+      <c r="AE33" s="42" t="n"/>
+      <c r="AF33" s="42" t="n"/>
+      <c r="AG33" s="40" t="n"/>
+      <c r="AH33" s="45" t="n"/>
     </row>
     <row r="34" ht="14.4" customHeight="1">
       <c r="A34" s="10" t="n">
@@ -2759,16 +3033,28 @@
           <t>Ball Valve with Pneumatic actuator</t>
         </is>
       </c>
-      <c r="N36" s="13" t="n"/>
-      <c r="O36" s="10" t="n"/>
-      <c r="P36" s="13" t="n"/>
+      <c r="N36" s="13" t="inlineStr">
+        <is>
+          <t>edo</t>
+        </is>
+      </c>
+      <c r="O36" s="10" t="inlineStr">
+        <is>
+          <t>tony</t>
+        </is>
+      </c>
+      <c r="P36" s="13" t="inlineStr">
+        <is>
+          <t>cartoncesso</t>
+        </is>
+      </c>
       <c r="Q36" s="18" t="n"/>
       <c r="R36" s="10" t="n"/>
       <c r="S36" s="10" t="n"/>
       <c r="T36" s="10" t="n"/>
-      <c r="U36" s="10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
+      <c r="U36" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
         </is>
       </c>
       <c r="V36" s="10" t="n"/>
@@ -2816,13 +3102,17 @@
         </is>
       </c>
       <c r="N37" s="13" t="n"/>
-      <c r="O37" s="10" t="n"/>
-      <c r="P37" s="13" t="n"/>
+      <c r="O37" s="11" t="n"/>
+      <c r="P37" s="23" t="n"/>
       <c r="Q37" s="18" t="n"/>
       <c r="R37" s="10" t="n"/>
       <c r="S37" s="10" t="n"/>
       <c r="T37" s="10" t="n"/>
-      <c r="U37" s="10" t="n"/>
+      <c r="U37" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Flanged</t>
+        </is>
+      </c>
       <c r="V37" s="10" t="n"/>
       <c r="W37" s="10" t="n"/>
       <c r="X37" s="13" t="n"/>

</xml_diff>